<commit_message>
...cittadinanza e richiesta Pietro Pirotto
</commit_message>
<xml_diff>
--- a/TemplateExportAnagraficaPerAnno.xlsx
+++ b/TemplateExportAnagraficaPerAnno.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10917"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolacardi/Cartelle/localhost/waldorf/swapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0242C0C-52B5-0D47-B1CB-EF07C3873B1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F32783BD-3D91-4C4A-90E6-D2E6A11E0B25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="1140" windowWidth="27180" windowHeight="14700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-280" yWindow="500" windowWidth="27180" windowHeight="14700" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AnagraficheComplete" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="81">
   <si>
     <t>2019-20</t>
   </si>
@@ -261,6 +261,9 @@
   </si>
   <si>
     <t>Classe Anno Precedente</t>
+  </si>
+  <si>
+    <t>Nazionalità</t>
   </si>
 </sst>
 </file>
@@ -473,7 +476,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -529,6 +532,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -598,8 +604,11 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -912,7 +921,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BY5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="5" topLeftCell="U6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
@@ -992,80 +1001,80 @@
       <c r="A2" s="20"/>
     </row>
     <row r="3" spans="1:77" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="28"/>
-      <c r="K3" s="26" t="s">
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="29"/>
+      <c r="K3" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L3" s="27"/>
-      <c r="M3" s="27"/>
-      <c r="N3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="29"/>
       <c r="O3" s="3"/>
-      <c r="S3" s="26" t="s">
+      <c r="S3" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="T3" s="27"/>
-      <c r="U3" s="28"/>
-      <c r="V3" s="26" t="s">
+      <c r="T3" s="28"/>
+      <c r="U3" s="29"/>
+      <c r="V3" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="W3" s="27"/>
-      <c r="X3" s="27"/>
-      <c r="Y3" s="28"/>
-      <c r="Z3" s="26" t="s">
+      <c r="W3" s="28"/>
+      <c r="X3" s="28"/>
+      <c r="Y3" s="29"/>
+      <c r="Z3" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="AA3" s="27"/>
-      <c r="AB3" s="27"/>
-      <c r="AC3" s="35"/>
-      <c r="AD3" s="32" t="s">
+      <c r="AA3" s="28"/>
+      <c r="AB3" s="28"/>
+      <c r="AC3" s="36"/>
+      <c r="AD3" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="AE3" s="33"/>
-      <c r="AF3" s="33"/>
-      <c r="AG3" s="33"/>
-      <c r="AH3" s="33"/>
-      <c r="AI3" s="34"/>
-      <c r="AJ3" s="44" t="s">
+      <c r="AE3" s="34"/>
+      <c r="AF3" s="34"/>
+      <c r="AG3" s="34"/>
+      <c r="AH3" s="34"/>
+      <c r="AI3" s="35"/>
+      <c r="AJ3" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="AK3" s="32" t="s">
+      <c r="AK3" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="AL3" s="33"/>
-      <c r="AM3" s="33"/>
-      <c r="AN3" s="34"/>
-      <c r="BB3" s="29" t="s">
+      <c r="AL3" s="34"/>
+      <c r="AM3" s="34"/>
+      <c r="AN3" s="35"/>
+      <c r="BB3" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="BC3" s="30"/>
-      <c r="BD3" s="30"/>
-      <c r="BE3" s="31"/>
-      <c r="BG3" s="21" t="s">
+      <c r="BC3" s="31"/>
+      <c r="BD3" s="31"/>
+      <c r="BE3" s="32"/>
+      <c r="BG3" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="BH3" s="21"/>
-      <c r="BI3" s="21"/>
-      <c r="BJ3" s="21"/>
-      <c r="BK3" s="21"/>
-      <c r="BN3" s="22" t="s">
+      <c r="BH3" s="22"/>
+      <c r="BI3" s="22"/>
+      <c r="BJ3" s="22"/>
+      <c r="BK3" s="22"/>
+      <c r="BN3" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="BO3" s="22"/>
-      <c r="BP3" s="22"/>
-      <c r="BQ3" s="22"/>
-      <c r="BS3" s="23" t="s">
+      <c r="BO3" s="23"/>
+      <c r="BP3" s="23"/>
+      <c r="BQ3" s="23"/>
+      <c r="BS3" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="BT3" s="24"/>
-      <c r="BU3" s="24"/>
-      <c r="BV3" s="24"/>
-      <c r="BW3" s="25"/>
+      <c r="BT3" s="25"/>
+      <c r="BU3" s="25"/>
+      <c r="BV3" s="25"/>
+      <c r="BW3" s="26"/>
     </row>
     <row r="5" spans="1:77" s="10" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
@@ -1322,11 +1331,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AR5"/>
+  <dimension ref="A1:AT5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1347,89 +1354,91 @@
     <col min="15" max="15" width="10.5" style="1" customWidth="1"/>
     <col min="16" max="16" width="30.5" customWidth="1"/>
     <col min="17" max="17" width="4.6640625" customWidth="1"/>
-    <col min="18" max="18" width="10.5" customWidth="1"/>
-    <col min="19" max="19" width="20.5" customWidth="1"/>
-    <col min="20" max="20" width="30.6640625" customWidth="1"/>
-    <col min="21" max="21" width="21.5" customWidth="1"/>
-    <col min="22" max="22" width="6.33203125" customWidth="1"/>
-    <col min="23" max="23" width="4.6640625" customWidth="1"/>
-    <col min="24" max="24" width="9.5" customWidth="1"/>
-    <col min="26" max="26" width="33.5" customWidth="1"/>
-    <col min="27" max="27" width="10.5" style="1" customWidth="1"/>
-    <col min="28" max="28" width="24.5" customWidth="1"/>
-    <col min="29" max="29" width="4.6640625" customWidth="1"/>
-    <col min="30" max="30" width="10.6640625" customWidth="1"/>
-    <col min="31" max="31" width="20.1640625" customWidth="1"/>
-    <col min="32" max="32" width="30.6640625" customWidth="1"/>
-    <col min="33" max="33" width="21.5" customWidth="1"/>
-    <col min="34" max="34" width="6.33203125" customWidth="1"/>
-    <col min="35" max="35" width="4.6640625" customWidth="1"/>
-    <col min="36" max="36" width="9.5" customWidth="1"/>
-    <col min="38" max="38" width="33.5" customWidth="1"/>
-    <col min="39" max="40" width="9.33203125" customWidth="1"/>
-    <col min="41" max="41" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="13" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="10.5" customWidth="1"/>
+    <col min="20" max="20" width="20.5" customWidth="1"/>
+    <col min="21" max="21" width="30.6640625" customWidth="1"/>
+    <col min="22" max="22" width="21.5" customWidth="1"/>
+    <col min="23" max="23" width="6.33203125" customWidth="1"/>
+    <col min="24" max="24" width="4.6640625" customWidth="1"/>
+    <col min="25" max="25" width="9.5" customWidth="1"/>
+    <col min="27" max="27" width="33.5" customWidth="1"/>
+    <col min="28" max="28" width="10.5" style="1" customWidth="1"/>
+    <col min="29" max="29" width="24.5" customWidth="1"/>
+    <col min="30" max="30" width="4.6640625" customWidth="1"/>
+    <col min="31" max="32" width="10.6640625" customWidth="1"/>
+    <col min="33" max="33" width="20.1640625" customWidth="1"/>
+    <col min="34" max="34" width="30.6640625" customWidth="1"/>
+    <col min="35" max="35" width="21.5" customWidth="1"/>
+    <col min="36" max="36" width="6.33203125" customWidth="1"/>
+    <col min="37" max="37" width="4.6640625" customWidth="1"/>
+    <col min="38" max="38" width="9.5" customWidth="1"/>
+    <col min="40" max="40" width="33.5" customWidth="1"/>
+    <col min="41" max="42" width="9.33203125" customWidth="1"/>
+    <col min="43" max="43" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:46" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="AO1" s="19" t="s">
+      <c r="AQ1" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="AP1" s="19" t="s">
+      <c r="AR1" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="AQ1" s="19" t="s">
+      <c r="AS1" s="19" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:44" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AO2" s="18" t="s">
+    <row r="2" spans="1:46" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AQ2" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="AP2" s="18" t="s">
+      <c r="AR2" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="AQ2" s="19" t="s">
+      <c r="AS2" s="19" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="O3" s="41" t="s">
+    <row r="3" spans="1:46" x14ac:dyDescent="0.2">
+      <c r="O3" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="P3" s="42"/>
-      <c r="Q3" s="42"/>
-      <c r="R3" s="43"/>
-      <c r="T3" s="36" t="s">
+      <c r="P3" s="43"/>
+      <c r="Q3" s="43"/>
+      <c r="R3" s="44"/>
+      <c r="S3" s="45"/>
+      <c r="U3" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="U3" s="36"/>
-      <c r="V3" s="36"/>
-      <c r="W3" s="36"/>
-      <c r="X3" s="36"/>
-      <c r="AA3" s="37" t="s">
+      <c r="V3" s="37"/>
+      <c r="W3" s="37"/>
+      <c r="X3" s="37"/>
+      <c r="Y3" s="37"/>
+      <c r="AB3" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="AB3" s="37"/>
-      <c r="AC3" s="37"/>
-      <c r="AD3" s="37"/>
-      <c r="AF3" s="38" t="s">
+      <c r="AC3" s="38"/>
+      <c r="AD3" s="38"/>
+      <c r="AE3" s="38"/>
+      <c r="AF3" s="46"/>
+      <c r="AH3" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="AG3" s="39"/>
-      <c r="AH3" s="39"/>
-      <c r="AI3" s="39"/>
+      <c r="AI3" s="40"/>
       <c r="AJ3" s="40"/>
-      <c r="AO3" s="18"/>
-      <c r="AP3" s="18" t="s">
+      <c r="AK3" s="40"/>
+      <c r="AL3" s="41"/>
+      <c r="AQ3" s="18"/>
+      <c r="AR3" s="18" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:44" s="10" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:46" s="10" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>10</v>
       </c>
@@ -1485,90 +1494,96 @@
         <v>17</v>
       </c>
       <c r="S5" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="T5" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="T5" s="12" t="s">
+      <c r="U5" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="U5" s="12" t="s">
+      <c r="V5" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="V5" s="12" t="s">
+      <c r="W5" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="W5" s="12" t="s">
+      <c r="X5" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="X5" s="12" t="s">
+      <c r="Y5" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="Y5" s="12" t="s">
+      <c r="Z5" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="Z5" s="12" t="s">
+      <c r="AA5" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="AA5" s="15" t="s">
+      <c r="AB5" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="AB5" s="13" t="s">
+      <c r="AC5" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="AC5" s="13" t="s">
+      <c r="AD5" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="AD5" s="13" t="s">
+      <c r="AE5" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="AE5" s="13" t="s">
+      <c r="AF5" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="AG5" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="AF5" s="13" t="s">
+      <c r="AH5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="AG5" s="13" t="s">
+      <c r="AI5" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="AH5" s="13" t="s">
+      <c r="AJ5" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="AI5" s="13" t="s">
+      <c r="AK5" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="AJ5" s="13" t="s">
+      <c r="AL5" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="AK5" s="13" t="s">
+      <c r="AM5" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="AL5" s="13" t="s">
+      <c r="AN5" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="AM5" s="12" t="s">
+      <c r="AO5" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="AN5" s="13" t="s">
+      <c r="AP5" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="AO5" s="4" t="s">
+      <c r="AQ5" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="AP5" s="4" t="s">
+      <c r="AR5" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="AQ5" s="4" t="s">
+      <c r="AS5" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="AR5" s="4" t="s">
+      <c r="AT5" s="4" t="s">
         <v>70</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="4">
-    <mergeCell ref="T3:X3"/>
-    <mergeCell ref="AA3:AD3"/>
-    <mergeCell ref="AF3:AJ3"/>
+    <mergeCell ref="U3:Y3"/>
+    <mergeCell ref="AB3:AE3"/>
+    <mergeCell ref="AH3:AL3"/>
     <mergeCell ref="O3:R3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>